<commit_message>
add more data to daily_submission_stats and update graph
</commit_message>
<xml_diff>
--- a/insights/1/2019 DAY 1/daily_submission_stats.xlsx
+++ b/insights/1/2019 DAY 1/daily_submission_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ioi_project\ioi-grant\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ioi_project\ioi-grant\insights\1\2019 DAY 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{F1AC037A-A1FA-4330-98EE-3A9192980CD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21EA1BD6-7E8C-4486-96EE-F4668AEBFFE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019 DAY 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="27">
   <si>
     <t>task</t>
   </si>
@@ -84,11 +84,29 @@
   <si>
     <t>05:00</t>
   </si>
+  <si>
+    <t>rect</t>
+  </si>
+  <si>
+    <t>shoes</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>score &gt; 0</t>
+  </si>
+  <si>
+    <t>score &gt; 20</t>
+  </si>
+  <si>
+    <t>score &gt; 50</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -566,7 +584,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,6 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -670,13 +689,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Day</a:t>
+              <a:t>Day 1</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 1</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -719,7 +733,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Task 2</c:v>
+            <c:v>rect</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -735,7 +749,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$5:$K$5</c:f>
+              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -821,7 +835,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Task 3</c:v>
+            <c:v>shoes</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -837,7 +851,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$5:$K$5</c:f>
+              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -923,7 +937,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Task 4</c:v>
+            <c:v>split</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -939,7 +953,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$5:$K$5</c:f>
+              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1018,6 +1032,317 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-C805-4EE3-840A-DC792B2AEAFC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>rect0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>00:30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>01:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>01:30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>02:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>02:30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>03:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>03:30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>04:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>04:30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>05:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2019 DAY 1'!$B$9:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>308</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1D83-486F-BABA-85CBDE037D29}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>shoes0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>00:30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>01:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>01:30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>02:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>02:30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>03:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>03:30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>04:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>04:30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>05:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2019 DAY 1'!$B$10:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>163</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>234</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>155</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1D83-486F-BABA-85CBDE037D29}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>split0</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>00:30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>01:00</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>01:30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>02:00</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>02:30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>03:00</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>03:30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>04:00</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>04:30</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>05:00</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2019 DAY 1'!$B$11:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>164</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>287</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1D83-486F-BABA-85CBDE037D29}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1783,16 +2108,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2116,11 +2441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2161,8 +2486,8 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2</v>
+      <c r="A2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>24</v>
@@ -2196,8 +2521,8 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>3</v>
+      <c r="A3" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>194</v>
@@ -2231,8 +2556,8 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>4</v>
+      <c r="A4" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>13</v>
@@ -2295,6 +2620,537 @@
         <v>19</v>
       </c>
       <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <v>47</v>
+      </c>
+      <c r="E9" s="1">
+        <v>72</v>
+      </c>
+      <c r="F9" s="1">
+        <v>87</v>
+      </c>
+      <c r="G9" s="1">
+        <v>101</v>
+      </c>
+      <c r="H9" s="1">
+        <v>108</v>
+      </c>
+      <c r="I9" s="1">
+        <v>143</v>
+      </c>
+      <c r="J9" s="1">
+        <v>179</v>
+      </c>
+      <c r="K9" s="1">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1">
+        <v>163</v>
+      </c>
+      <c r="C10" s="1">
+        <v>234</v>
+      </c>
+      <c r="D10" s="1">
+        <v>294</v>
+      </c>
+      <c r="E10" s="1">
+        <v>172</v>
+      </c>
+      <c r="F10" s="1">
+        <v>216</v>
+      </c>
+      <c r="G10" s="1">
+        <v>137</v>
+      </c>
+      <c r="H10" s="1">
+        <v>167</v>
+      </c>
+      <c r="I10" s="1">
+        <v>121</v>
+      </c>
+      <c r="J10" s="1">
+        <v>115</v>
+      </c>
+      <c r="K10" s="1">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1">
+        <v>62</v>
+      </c>
+      <c r="E11" s="1">
+        <v>95</v>
+      </c>
+      <c r="F11" s="1">
+        <v>144</v>
+      </c>
+      <c r="G11" s="1">
+        <v>148</v>
+      </c>
+      <c r="H11" s="1">
+        <v>165</v>
+      </c>
+      <c r="I11" s="1">
+        <v>211</v>
+      </c>
+      <c r="J11" s="1">
+        <v>164</v>
+      </c>
+      <c r="K11" s="1">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1">
+        <v>19</v>
+      </c>
+      <c r="E16" s="1">
+        <v>52</v>
+      </c>
+      <c r="F16" s="1">
+        <v>58</v>
+      </c>
+      <c r="G16" s="1">
+        <v>62</v>
+      </c>
+      <c r="H16" s="1">
+        <v>73</v>
+      </c>
+      <c r="I16" s="1">
+        <v>84</v>
+      </c>
+      <c r="J16" s="1">
+        <v>116</v>
+      </c>
+      <c r="K16" s="1">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1">
+        <v>55</v>
+      </c>
+      <c r="C17" s="1">
+        <v>107</v>
+      </c>
+      <c r="D17" s="1">
+        <v>169</v>
+      </c>
+      <c r="E17" s="1">
+        <v>100</v>
+      </c>
+      <c r="F17" s="1">
+        <v>114</v>
+      </c>
+      <c r="G17" s="1">
+        <v>63</v>
+      </c>
+      <c r="H17" s="1">
+        <v>102</v>
+      </c>
+      <c r="I17" s="1">
+        <v>62</v>
+      </c>
+      <c r="J17" s="1">
+        <v>57</v>
+      </c>
+      <c r="K17" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1">
+        <v>4</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>15</v>
+      </c>
+      <c r="E18" s="1">
+        <v>23</v>
+      </c>
+      <c r="F18" s="1">
+        <v>64</v>
+      </c>
+      <c r="G18" s="1">
+        <v>65</v>
+      </c>
+      <c r="H18" s="1">
+        <v>66</v>
+      </c>
+      <c r="I18" s="1">
+        <v>99</v>
+      </c>
+      <c r="J18" s="1">
+        <v>62</v>
+      </c>
+      <c r="K18" s="1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
+      <c r="E23" s="1">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1">
+        <v>21</v>
+      </c>
+      <c r="G23" s="1">
+        <v>23</v>
+      </c>
+      <c r="H23" s="1">
+        <v>28</v>
+      </c>
+      <c r="I23" s="1">
+        <v>30</v>
+      </c>
+      <c r="J23" s="1">
+        <v>31</v>
+      </c>
+      <c r="K23" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1">
+        <v>4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1">
+        <v>52</v>
+      </c>
+      <c r="E24" s="1">
+        <v>27</v>
+      </c>
+      <c r="F24" s="1">
+        <v>27</v>
+      </c>
+      <c r="G24" s="1">
+        <v>15</v>
+      </c>
+      <c r="H24" s="1">
+        <v>26</v>
+      </c>
+      <c r="I24" s="1">
+        <v>11</v>
+      </c>
+      <c r="J24" s="1">
+        <v>13</v>
+      </c>
+      <c r="K24" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>2</v>
+      </c>
+      <c r="J25" s="1">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>